<commit_message>
tiger heli v2 progress
</commit_message>
<xml_diff>
--- a/Tiger-Heli/FrameCompare.xlsx
+++ b/Tiger-Heli/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\Tiger-Heli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE04BA8-EAC6-4722-B869-2319BA6AED0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC4DD72-80F4-4E19-B756-1891797FA2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14595" yWindow="3960" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>Place</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>X=239,243</t>
+  </si>
+  <si>
+    <t>Leave Helipad 2</t>
   </si>
 </sst>
 </file>
@@ -291,7 +294,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -312,6 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -636,7 +640,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -646,7 +650,7 @@
     <col min="4" max="4" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -671,12 +675,12 @@
         <v>87</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D13" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D14" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>24</v>
       </c>
@@ -692,7 +696,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>26</v>
       </c>
@@ -707,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>27</v>
       </c>
@@ -722,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>29</v>
       </c>
@@ -737,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>30</v>
       </c>
@@ -755,8 +759,12 @@
         <f>B7-B6</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>12247-11527</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>31</v>
       </c>
@@ -775,7 +783,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>32</v>
       </c>
@@ -794,7 +802,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>33</v>
       </c>
@@ -813,7 +821,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>34</v>
       </c>
@@ -832,13 +840,13 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>28</v>
       </c>
@@ -851,21 +859,30 @@
         <v>-</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="15">
+        <v>24488</v>
+      </c>
+      <c r="C14" s="15">
+        <v>24488</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>

</xml_diff>

<commit_message>
Tiger-heli - end input sooner, might be a few more frames that can be eeked out
</commit_message>
<xml_diff>
--- a/Tiger-Heli/FrameCompare.xlsx
+++ b/Tiger-Heli/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\Tiger-Heli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC4DD72-80F4-4E19-B756-1891797FA2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CF50E6-4828-4E63-BBFA-6AB2B85C4725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14595" yWindow="3960" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28095" yWindow="885" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>Place</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Leave Helipad 2</t>
+  </si>
+  <si>
+    <t>Leave Helipad 3</t>
   </si>
 </sst>
 </file>
@@ -640,7 +643,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -675,7 +678,7 @@
         <v>87</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D14" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D16" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -876,17 +879,35 @@
       <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
+      <c r="A15" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="15">
+        <v>36728</v>
+      </c>
+      <c r="C15" s="15">
+        <v>36728</v>
+      </c>
+      <c r="D15" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
+      <c r="A16" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="15">
+        <v>46875</v>
+      </c>
+      <c r="C16" s="15">
+        <v>47844</v>
+      </c>
+      <c r="D16" s="16">
+        <f t="shared" si="0"/>
+        <v>969</v>
+      </c>
       <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">

</xml_diff>